<commit_message>
home, search and investigation page changes
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Parag\Git\IVFmilan\src\main\java\com_Milan_TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="155">
   <si>
     <t>PatientName</t>
   </si>
@@ -456,9 +456,6 @@
     <t>You can add only one cycle for same visit.</t>
   </si>
   <si>
-    <t>Shaila</t>
-  </si>
-  <si>
     <t>ICSI</t>
   </si>
   <si>
@@ -502,6 +499,15 @@
   </si>
   <si>
     <t>8</t>
+  </si>
+  <si>
+    <t>Record saved successfully</t>
+  </si>
+  <si>
+    <t>Laxmi</t>
+  </si>
+  <si>
+    <t>Ms.Nargis</t>
   </si>
 </sst>
 </file>
@@ -870,7 +876,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -912,16 +918,16 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="48.7109375" collapsed="true"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="48.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="10" customFormat="1">
@@ -967,13 +973,13 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>121</v>
+      <c r="A7" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
-        <v>137</v>
+      <c r="A8" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1013,7 +1019,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:1">
@@ -1023,7 +1029,7 @@
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:1">
@@ -1044,6 +1050,11 @@
     <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1063,7 +1074,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1098,14 +1109,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="15" width="13.7109375" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" style="15" width="13.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="10.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="15" width="12.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="15" width="29.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.85546875" collapsed="true"/>
-    <col min="9" max="16384" style="15" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="13.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.85546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="15" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="14" customFormat="1">
@@ -1260,10 +1271,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="3" max="3" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
@@ -1426,20 +1437,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1">
@@ -1939,10 +1950,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="71.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="10" customFormat="1">
@@ -2019,17 +2030,17 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="54.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="4" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="38.28515625" collapsed="true"/>
+    <col min="2" max="2" width="54.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="38.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="10" customFormat="1">
@@ -2040,7 +2051,7 @@
         <v>119</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>128</v>
@@ -2064,7 +2075,7 @@
         <v>134</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>135</v>
@@ -2081,10 +2092,10 @@
         <v>128</v>
       </c>
       <c r="D2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F2" t="s">
         <v>130</v>
@@ -2093,7 +2104,7 @@
         <v>131</v>
       </c>
       <c r="H2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I2" t="s">
         <v>130</v>
@@ -2102,10 +2113,10 @@
         <v>131</v>
       </c>
       <c r="K2" t="s">
+        <v>151</v>
+      </c>
+      <c r="L2" t="s">
         <v>152</v>
-      </c>
-      <c r="L2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -2116,16 +2127,19 @@
         <v>129</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I3" t="s">
-        <v>146</v>
+        <v>145</v>
+      </c>
+      <c r="L3" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -2136,13 +2150,13 @@
         <v>130</v>
       </c>
       <c r="D4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -2150,13 +2164,13 @@
         <v>127</v>
       </c>
       <c r="C5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -2201,15 +2215,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>147</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2217,7 +2231,7 @@
         <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:2">

</xml_diff>

<commit_message>
Invesigation and opucycle changes
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="5" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="159">
   <si>
     <t>PatientName</t>
   </si>
@@ -442,9 +442,6 @@
     <t>Oocyte Recipient</t>
   </si>
   <si>
-    <t>Fash message</t>
-  </si>
-  <si>
     <t>You can add only one cycle for same visit.</t>
   </si>
   <si>
@@ -493,9 +490,6 @@
     <t>8</t>
   </si>
   <si>
-    <t>Record saved successfully</t>
-  </si>
-  <si>
     <t>Laxmi</t>
   </si>
   <si>
@@ -505,9 +499,6 @@
     <t>,17 BETAESTRADIOL,foodAllergy,SkinAllergy,smokeAllergy</t>
   </si>
   <si>
-    <t>Nandita</t>
-  </si>
-  <si>
     <t>Allergies</t>
   </si>
   <si>
@@ -518,6 +509,18 @@
   </si>
   <si>
     <t>526 IVF - 1ST CYCLE - International Package - OMAN</t>
+  </si>
+  <si>
+    <t>Fashmessage</t>
+  </si>
+  <si>
+    <t>Record saved successfully.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geeta </t>
+  </si>
+  <si>
+    <t>Record deleted successfully.</t>
   </si>
 </sst>
 </file>
@@ -941,7 +944,7 @@
   <sheetData>
     <row r="1" spans="4:5">
       <c r="D1" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>68</v>
@@ -954,7 +957,7 @@
     </row>
     <row r="3" spans="4:5">
       <c r="E3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -969,7 +972,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -991,7 +994,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1022,12 +1025,12 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1067,12 +1070,12 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -1998,7 +2001,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="71.66796875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="71.7109375" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
@@ -2078,8 +2081,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2099,7 +2102,7 @@
         <v>117</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>125</v>
@@ -2123,10 +2126,10 @@
         <v>131</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -2140,10 +2143,10 @@
         <v>125</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F2" t="s">
         <v>127</v>
@@ -2152,7 +2155,7 @@
         <v>128</v>
       </c>
       <c r="H2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I2" t="s">
         <v>127</v>
@@ -2161,10 +2164,10 @@
         <v>128</v>
       </c>
       <c r="K2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L2" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -2175,19 +2178,19 @@
         <v>126</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -2198,13 +2201,16 @@
         <v>127</v>
       </c>
       <c r="D4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H4" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="L4" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -2212,13 +2218,13 @@
         <v>123</v>
       </c>
       <c r="C5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -2231,7 +2237,7 @@
     </row>
     <row r="7" spans="1:12">
       <c r="B7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C7" t="s">
         <v>130</v>
@@ -2239,7 +2245,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="B8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C8" t="s">
         <v>131</v>
@@ -2261,7 +2267,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2271,10 +2277,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>143</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2282,7 +2288,7 @@
         <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:2">

</xml_diff>

<commit_message>
Changes in diffrent pages
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Parag\Git\IVFmilan\src\main\java\com_Milan_TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="5" r:id="rId1"/>
@@ -20,8 +20,9 @@
     <sheet name="SexualHistory" sheetId="3" r:id="rId6"/>
     <sheet name="pastMedicationHistory" sheetId="4" r:id="rId7"/>
     <sheet name="Investigation" sheetId="8" r:id="rId8"/>
-    <sheet name="Investigationlist" sheetId="9" r:id="rId9"/>
-    <sheet name="Allergies" sheetId="10" r:id="rId10"/>
+    <sheet name="CycleList" sheetId="11" r:id="rId9"/>
+    <sheet name="Investigationlist" sheetId="9" r:id="rId10"/>
+    <sheet name="Allergies" sheetId="10" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="ERLinked">Investigation!$I$2:$I$3</definedName>
@@ -34,7 +35,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="160">
   <si>
     <t>PatientName</t>
   </si>
@@ -521,6 +522,9 @@
   </si>
   <si>
     <t>Record deleted successfully.</t>
+  </si>
+  <si>
+    <t>ListTitle</t>
   </si>
 </sst>
 </file>
@@ -890,7 +894,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -930,6 +934,78 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A11">
+      <formula1>IVFPackage</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B8">
+      <formula1>INDIRECT($A2)</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:E3"/>
   <sheetViews>
@@ -939,7 +1015,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
+    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:5">
@@ -977,8 +1053,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="48.7109375" collapsed="true"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="48.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="10" customFormat="1">
@@ -1125,7 +1201,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1160,14 +1236,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="15" width="13.7109375" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" style="15" width="13.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="10.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="15" width="12.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="15" width="29.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.85546875" collapsed="true"/>
-    <col min="9" max="16384" style="15" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="13.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.85546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="15" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="14" customFormat="1">
@@ -1322,10 +1398,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="3" max="3" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
@@ -1482,26 +1558,26 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1">
@@ -1552,16 +1628,16 @@
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" t="s">
@@ -1570,10 +1646,10 @@
       <c r="F2" t="s">
         <v>38</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>0</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <v>0</v>
       </c>
       <c r="I2" t="s">
@@ -1593,16 +1669,16 @@
       </c>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" t="s">
@@ -1611,10 +1687,10 @@
       <c r="F3" t="s">
         <v>39</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>1</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <v>1</v>
       </c>
       <c r="I3" t="s">
@@ -1634,25 +1710,25 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>2</v>
       </c>
       <c r="F4" t="s">
         <v>40</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>2</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <v>2</v>
       </c>
       <c r="K4" t="s">
@@ -1660,25 +1736,25 @@
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>3</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>3</v>
       </c>
       <c r="F5" t="s">
         <v>41</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>3</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <v>3</v>
       </c>
       <c r="K5" t="s">
@@ -1686,22 +1762,22 @@
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>4</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>4</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>4</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
         <v>4</v>
       </c>
       <c r="K6" t="s">
@@ -1709,22 +1785,22 @@
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>5</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>5</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>5</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <v>5</v>
       </c>
       <c r="K7" t="s">
@@ -1732,255 +1808,255 @@
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>6</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>6</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>6</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>6</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>7</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>7</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>7</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>7</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>8</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>8</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>8</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>8</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="2">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>9</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>9</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>9</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>9</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>10</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>10</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>10</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>10</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13">
+      <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>11</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>11</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>11</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>11</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="2">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14">
+      <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>12</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15">
+      <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>13</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="2">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16">
+      <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>14</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="2">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17">
+      <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>15</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="2">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18">
+      <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>16</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19">
+      <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>17</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="2">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20">
+      <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>18</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="2">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21">
+      <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22">
+      <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23">
+      <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="2">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24">
+      <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="2">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25">
+      <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="2">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26">
+      <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27">
+      <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="2">
         <v>25</v>
       </c>
     </row>
@@ -2001,10 +2077,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="71.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="10" customFormat="1">
@@ -2081,17 +2157,17 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="4" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="38.28515625" collapsed="true"/>
+    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="38.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="10" customFormat="1">
@@ -2264,72 +2340,21 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>131</v>
+    <row r="1" spans="1:1">
+      <c r="A1" s="7" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A11">
-      <formula1>IVFPackage</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B8">
-      <formula1>INDIRECT($A2)</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
investigationOPU and cycle list pages changes
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Parag\Git\IVFmilan\src\main\java\com_Milan_TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="177">
   <si>
     <t>PatientName</t>
   </si>
@@ -530,7 +530,52 @@
     <t>Aradhya</t>
   </si>
   <si>
-    <t>Cycle List</t>
+    <t>New Cycle</t>
+  </si>
+  <si>
+    <t>ProtocolName</t>
+  </si>
+  <si>
+    <t>ARTtype</t>
+  </si>
+  <si>
+    <t>ARTSubtype</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>Agonist Depot</t>
+  </si>
+  <si>
+    <t>Antagonist</t>
+  </si>
+  <si>
+    <t>Flare</t>
+  </si>
+  <si>
+    <t>GnRh Long Protocol</t>
+  </si>
+  <si>
+    <t>Minimal Stimulation</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Recipient Antagonist</t>
+  </si>
+  <si>
+    <t>Recipient Depot</t>
+  </si>
+  <si>
+    <t>Ultrashort</t>
+  </si>
+  <si>
+    <t>Soft Protocol</t>
+  </si>
+  <si>
+    <t>Agonist Daily</t>
   </si>
 </sst>
 </file>
@@ -906,7 +951,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -955,7 +1000,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1022,12 +1067,12 @@
   <dimension ref="D1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:5">
@@ -1060,13 +1105,13 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="48.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="48.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="10" customFormat="1">
@@ -1218,7 +1263,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1253,14 +1298,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="13.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.85546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="15" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="15" width="13.7109375" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" style="15" width="13.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="10.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="15" width="12.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="15" width="29.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.85546875" collapsed="true"/>
+    <col min="9" max="16384" style="15" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="14" customFormat="1">
@@ -1415,10 +1460,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
@@ -1581,20 +1626,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1">
@@ -2094,10 +2139,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="71.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="10" customFormat="1">
@@ -2175,16 +2220,16 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="38.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="4" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="38.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="10" customFormat="1">
@@ -2357,22 +2402,98 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.78125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.39453125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.85546875" collapsed="true"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="C3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D3" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="C4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="C5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="C6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="C7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="C8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="C9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="C10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="C11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="C12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="C13" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cyclepage cycle list page changes
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Parag\Git\IVFmilan\src\main\java\com_Milan_TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="5" r:id="rId1"/>
@@ -21,8 +21,9 @@
     <sheet name="pastMedicationHistory" sheetId="4" r:id="rId7"/>
     <sheet name="Investigation" sheetId="8" r:id="rId8"/>
     <sheet name="CycleList" sheetId="11" r:id="rId9"/>
-    <sheet name="Investigationlist" sheetId="9" r:id="rId10"/>
-    <sheet name="Allergies" sheetId="10" r:id="rId11"/>
+    <sheet name="Diagnosis" sheetId="12" r:id="rId10"/>
+    <sheet name="Investigationlist" sheetId="9" r:id="rId11"/>
+    <sheet name="Allergies" sheetId="10" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="ERLinked">Investigation!$I$2:$I$3</definedName>
@@ -35,7 +36,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="186">
   <si>
     <t>PatientName</t>
   </si>
@@ -54,14 +55,6 @@
     <t>BPSystolicval</t>
   </si>
   <si>
-    <t>Ms.Hema
-PUN-GEM-2018-04-005</t>
-  </si>
-  <si>
-    <t>Mr.Ram
-PUN-GEM-2018-04-006</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pratiksha </t>
   </si>
   <si>
@@ -542,9 +535,44 @@
     <t>ARTSubtype</t>
   </si>
   <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Favourite Diagnosis Deleted Successfully</t>
+  </si>
+  <si>
+    <t>Codevalue</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Record saved successfully!"</t>
+  </si>
+  <si>
+    <t>favoritedelete</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr.Ram
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms.Hema
+</t>
+  </si>
+  <si>
+    <t>SiemenSize</t>
+  </si>
+  <si>
+    <t>SiemenName</t>
+  </si>
+  <si>
     <t>Select</t>
   </si>
   <si>
+    <t>Agonist Daily</t>
+  </si>
+  <si>
     <t>Agonist Depot</t>
   </si>
   <si>
@@ -575,7 +603,7 @@
     <t>Soft Protocol</t>
   </si>
   <si>
-    <t>Agonist Daily</t>
+    <t>SpermName</t>
   </si>
 </sst>
 </file>
@@ -639,7 +667,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -662,6 +690,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -946,42 +977,42 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
       <c r="A1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
         <v>69</v>
-      </c>
-      <c r="C3" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -991,6 +1022,51 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="38" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -1000,53 +1076,53 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1062,7 +1138,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:E3"/>
   <sheetViews>
@@ -1072,25 +1148,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
+    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:5">
       <c r="D1" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="4:5">
       <c r="E2" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="4:5">
       <c r="E3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1105,13 +1181,13 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="48.7109375" collapsed="true"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="48.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="10" customFormat="1">
@@ -1119,131 +1195,131 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="19" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>3</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30">
+      <c r="A9" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30">
+      <c r="A10" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1263,22 +1339,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1298,149 +1374,149 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="15" width="13.7109375" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" style="15" width="13.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="10.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="15" width="12.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="15" width="29.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.85546875" collapsed="true"/>
-    <col min="9" max="16384" style="15" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="13.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.85546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="15" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="14" customFormat="1">
       <c r="A1" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>75</v>
-      </c>
       <c r="E1" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C3" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="15" t="s">
-        <v>91</v>
-      </c>
       <c r="E3" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F3" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="16" t="s">
         <v>96</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>94</v>
-      </c>
       <c r="E4" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1460,18 +1536,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="3" max="3" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
       <c r="A1" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>2</v>
@@ -1480,13 +1556,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1497,10 +1573,10 @@
         <v>180</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2" s="3">
         <v>59</v>
@@ -1521,10 +1597,10 @@
         <v>170</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2">
         <v>60</v>
@@ -1545,10 +1621,10 @@
         <v>160</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4" s="2">
         <v>80</v>
@@ -1569,10 +1645,10 @@
         <v>150</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" s="2">
         <v>99</v>
@@ -1593,10 +1669,10 @@
         <v>100</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E6" s="2">
         <v>101</v>
@@ -1626,67 +1702,67 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1">
       <c r="A1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="M1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="O1" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -1703,10 +1779,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
         <v>36</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
       </c>
       <c r="G2" s="2">
         <v>0</v>
@@ -1715,19 +1791,19 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
         <v>42</v>
       </c>
-      <c r="J2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K2" t="s">
-        <v>44</v>
-      </c>
       <c r="L2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="O2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -1744,10 +1820,10 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
         <v>37</v>
-      </c>
-      <c r="F3" t="s">
-        <v>39</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
@@ -1756,19 +1832,19 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" t="s">
         <v>43</v>
       </c>
-      <c r="J3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" t="s">
-        <v>45</v>
-      </c>
       <c r="L3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -1785,7 +1861,7 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G4" s="2">
         <v>2</v>
@@ -1794,7 +1870,7 @@
         <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1811,7 +1887,7 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G5" s="2">
         <v>3</v>
@@ -1820,7 +1896,7 @@
         <v>3</v>
       </c>
       <c r="K5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1843,7 +1919,7 @@
         <v>4</v>
       </c>
       <c r="K6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1866,7 +1942,7 @@
         <v>5</v>
       </c>
       <c r="K7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -2139,64 +2215,64 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="71.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="10" customFormat="1">
       <c r="A1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>52</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="10" customFormat="1">
       <c r="A2" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2220,173 +2296,173 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="4" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="38.28515625" collapsed="true"/>
+    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="38.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="10" customFormat="1">
       <c r="A1" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>116</v>
-      </c>
       <c r="C1" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="I1" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>130</v>
-      </c>
       <c r="K1" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" t="s">
         <v>124</v>
       </c>
-      <c r="D2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F2" t="s">
-        <v>126</v>
-      </c>
       <c r="G2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="L2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="B3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="L3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="B4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="L4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="B5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="B6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="B7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="B8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2402,98 +2478,116 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.78125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.39453125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>156</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>173</v>
+      </c>
+      <c r="D2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="C3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="C4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5" t="s">
         <v>176</v>
       </c>
-      <c r="D3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="C4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="C5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+    </row>
+    <row r="6" spans="1:7">
       <c r="C6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="C7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="C8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="C9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="C10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="C11" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="C12" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="C13" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cyclelist Addictions Emr Home page and others are modified
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Parag\Git\IVFmilan\src\main\java\com_Milan_TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="189">
   <si>
     <t>PatientName</t>
   </si>
@@ -542,9 +542,6 @@
   </si>
   <si>
     <t>favoritedelete</t>
-  </si>
-  <si>
-    <t>105</t>
   </si>
   <si>
     <t xml:space="preserve">Mr.Ram
@@ -604,6 +601,18 @@
   </si>
   <si>
     <t>Sudha</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>Partner+Donor</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -982,7 +991,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -1031,9 +1040,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1052,7 +1061,7 @@
         <v>162</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1076,7 +1085,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1148,7 +1157,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:5">
@@ -1180,14 +1189,14 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="48.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="48.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="10" customFormat="1">
@@ -1239,17 +1248,17 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30">
       <c r="A9" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30">
       <c r="A10" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1274,7 +1283,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1339,7 +1348,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1374,14 +1383,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="13.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.85546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="15" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="15" width="13.7109375" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" style="15" width="13.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="10.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="15" width="12.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="15" width="29.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.85546875" collapsed="true"/>
+    <col min="9" max="16384" style="15" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="14" customFormat="1">
@@ -1536,10 +1545,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
@@ -1702,20 +1711,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1">
@@ -2215,10 +2224,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="71.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="10" customFormat="1">
@@ -2301,11 +2310,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="38.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="4" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="38.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="10" customFormat="1">
@@ -2480,19 +2489,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.78125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2509,85 +2518,94 @@
         <v>154</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>170</v>
-      </c>
       <c r="G1" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>188</v>
       </c>
       <c r="C2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D2" t="s">
         <v>157</v>
       </c>
-      <c r="E2" t="s">
-        <v>89</v>
+      <c r="G2" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="C3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
         <v>157</v>
       </c>
+      <c r="G3" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="C4" t="s">
-        <v>173</v>
+        <v>172</v>
+      </c>
+      <c r="G4" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="C5" t="s">
-        <v>174</v>
+        <v>173</v>
+      </c>
+      <c r="G5" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="C6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="C7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="C8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="C9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="C10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="C11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="C12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="C13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
complaints investigation and xls data
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Parag\Git\IVFmilan\src\main\java\com_Milan_TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="189">
   <si>
     <t>PatientName</t>
   </si>
@@ -386,9 +386,6 @@
   </si>
   <si>
     <t>Searchresult</t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
   <si>
     <t>Nargis</t>
@@ -615,10 +612,7 @@
     <t>sourceofsperm</t>
   </si>
   <si>
-    <t>107</t>
-  </si>
-  <si>
-    <t>7</t>
+    <t>108</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +999,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -1054,33 +1048,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="1" max="1" width="38" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1099,53 +1093,53 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>138</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1171,12 +1165,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
+    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:5">
       <c r="D1" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>66</v>
@@ -1189,7 +1183,7 @@
     </row>
     <row r="3" spans="4:5">
       <c r="E3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1201,16 +1195,16 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="48.7109375" collapsed="true"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="48.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="10" customFormat="1">
@@ -1226,7 +1220,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1256,23 +1250,23 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="19" t="s">
-        <v>156</v>
+      <c r="A7" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30">
       <c r="A9" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30">
       <c r="A10" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1297,22 +1291,22 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:1">
@@ -1342,6 +1336,11 @@
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="19" t="s">
         <v>155</v>
       </c>
     </row>
@@ -1362,7 +1361,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1397,14 +1396,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="15" width="13.7109375" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" style="15" width="13.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="10.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="15" width="12.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="15" width="29.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.8359375" collapsed="true"/>
-    <col min="9" max="16384" style="15" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="13.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.85546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="15" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="14" customFormat="1">
@@ -1456,7 +1455,7 @@
         <v>95</v>
       </c>
       <c r="H2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1559,10 +1558,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="3" max="3" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
@@ -1719,26 +1718,26 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1">
@@ -2273,10 +2272,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="71.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="10" customFormat="1">
@@ -2359,11 +2358,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="4" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="38.28515625" collapsed="true"/>
+    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="38.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="10" customFormat="1">
@@ -2374,34 +2373,34 @@
         <v>113</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>127</v>
-      </c>
       <c r="K1" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -2409,118 +2408,118 @@
         <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G2" t="s">
         <v>123</v>
       </c>
-      <c r="G2" t="s">
-        <v>124</v>
-      </c>
       <c r="H2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I2" t="s">
+        <v>122</v>
+      </c>
+      <c r="J2" t="s">
         <v>123</v>
       </c>
-      <c r="J2" t="s">
-        <v>124</v>
-      </c>
       <c r="K2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="B3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="B4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="B5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="B6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="B7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="B8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2544,68 +2543,68 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>160</v>
-      </c>
       <c r="C1" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>169</v>
-      </c>
       <c r="G1" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="C3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H3" s="21" t="s">
         <v>106</v>
@@ -2613,7 +2612,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="C4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G4" t="s">
         <v>106</v>
@@ -2621,50 +2620,50 @@
     </row>
     <row r="5" spans="1:8">
       <c r="C5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="C6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="C7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="C8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="C9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="C10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="C11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="C12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="C13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addiction and emr page changes
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="5" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="198">
   <si>
     <t>PatientName</t>
   </si>
@@ -482,9 +482,6 @@
   </si>
   <si>
     <t>Allergies</t>
-  </si>
-  <si>
-    <t>Ms.Nandita</t>
   </si>
   <si>
     <t>All</t>
@@ -606,22 +603,40 @@
     <t>Partner+Donor</t>
   </si>
   <si>
+    <t>sourceofsperm</t>
+  </si>
+  <si>
+    <t>cyclenotfound</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>Cycle Already available</t>
+  </si>
+  <si>
+    <t>Neeta</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>sourceofsperm</t>
-  </si>
-  <si>
-    <t>108</t>
-  </si>
-  <si>
-    <t>cyclenotfound</t>
-  </si>
-  <si>
-    <t>109</t>
-  </si>
-  <si>
-    <t>0</t>
+    <t>Ejaculation</t>
+  </si>
+  <si>
+    <t>Surgical Extraction</t>
+  </si>
+  <si>
+    <t>Electrostimulation</t>
+  </si>
+  <si>
+    <t>Retrograde Ejaculation</t>
+  </si>
+  <si>
+    <t>Ms.Neeta </t>
+  </si>
+  <si>
+    <t>IndicationNames</t>
   </si>
   <si>
     <t>7</t>
@@ -634,7 +649,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -655,11 +670,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF545454"/>
-      <name val="Open_sansregular"/>
     </font>
     <font>
       <b/>
@@ -695,7 +705,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -717,11 +727,10 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1005,8 +1014,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1061,32 +1070,32 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>190</v>
+        <v>160</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1172,7 +1181,7 @@
   <dimension ref="D1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1207,10 +1216,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1232,7 +1241,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1263,22 +1272,22 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30">
       <c r="A9" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30">
       <c r="A10" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1303,17 +1312,17 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>146</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -1348,12 +1357,17 @@
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="19" t="s">
-        <v>155</v>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1402,8 +1416,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1467,7 +1481,7 @@
         <v>95</v>
       </c>
       <c r="H2" t="s">
-        <v>142</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2284,7 +2298,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="71.66796875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="71.7109375" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
@@ -2364,8 +2378,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2373,7 +2387,7 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
     <col min="4" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="38.28515625" collapsed="true"/>
   </cols>
   <sheetData>
@@ -2412,7 +2426,7 @@
         <v>139</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -2450,7 +2464,7 @@
         <v>142</v>
       </c>
       <c r="L2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -2473,7 +2487,7 @@
         <v>136</v>
       </c>
       <c r="L3" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -2493,7 +2507,7 @@
         <v>129</v>
       </c>
       <c r="L4" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -2510,7 +2524,7 @@
         <v>130</v>
       </c>
       <c r="L5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -2520,6 +2534,9 @@
       <c r="C6" t="s">
         <v>124</v>
       </c>
+      <c r="L6" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="7" spans="1:12">
       <c r="B7" t="s">
@@ -2531,7 +2548,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="B8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C8" t="s">
         <v>126</v>
@@ -2550,135 +2567,151 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.78125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="13.85546875" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>159</v>
-      </c>
       <c r="C1" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" t="s">
         <v>168</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="C3" t="s">
         <v>169</v>
       </c>
-      <c r="D2" t="s">
-        <v>156</v>
-      </c>
-      <c r="G2" t="s">
-        <v>169</v>
-      </c>
-      <c r="H2" s="21" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3" t="s">
+        <v>192</v>
+      </c>
+      <c r="G3" t="s">
+        <v>183</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="C4" t="s">
         <v>170</v>
       </c>
-      <c r="D3" t="s">
-        <v>156</v>
-      </c>
-      <c r="G3" t="s">
-        <v>184</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="C4" t="s">
-        <v>171</v>
+      <c r="F4" t="s">
+        <v>193</v>
       </c>
       <c r="G4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="C5" t="s">
+        <v>171</v>
+      </c>
+      <c r="F5" t="s">
+        <v>194</v>
+      </c>
+      <c r="G5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="C6" t="s">
         <v>172</v>
       </c>
-      <c r="G5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="C6" t="s">
+    </row>
+    <row r="7" spans="1:9">
+      <c r="C7" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="C7" t="s">
+    <row r="8" spans="1:9">
+      <c r="C8" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="C8" t="s">
+    <row r="9" spans="1:9">
+      <c r="C9" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="C9" t="s">
+    <row r="10" spans="1:9">
+      <c r="C10" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="C10" t="s">
+    <row r="11" spans="1:9">
+      <c r="C11" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="C11" t="s">
+    <row r="12" spans="1:9">
+      <c r="C12" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="C12" t="s">
+    <row r="13" spans="1:9">
+      <c r="C13" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="C13" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
slsxlogin,home complaints tests are modified
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Parag\Git\IVFmilan\src\main\java\com_Milan_TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="5" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="EMRPage" sheetId="7" r:id="rId3"/>
     <sheet name="Addictions" sheetId="6" r:id="rId4"/>
     <sheet name="Vitals" sheetId="2" r:id="rId5"/>
-    <sheet name="SexualHistory" sheetId="3" r:id="rId6"/>
-    <sheet name="pastMedicationHistory" sheetId="4" r:id="rId7"/>
-    <sheet name="Investigation" sheetId="8" r:id="rId8"/>
-    <sheet name="CycleList" sheetId="11" r:id="rId9"/>
-    <sheet name="Diagnosis" sheetId="12" r:id="rId10"/>
-    <sheet name="Investigationlist" sheetId="9" r:id="rId11"/>
-    <sheet name="Allergies" sheetId="10" r:id="rId12"/>
+    <sheet name="Complaints" sheetId="13" r:id="rId6"/>
+    <sheet name="SexualHistory" sheetId="3" r:id="rId7"/>
+    <sheet name="pastMedicationHistory" sheetId="4" r:id="rId8"/>
+    <sheet name="Investigation" sheetId="8" r:id="rId9"/>
+    <sheet name="CycleList" sheetId="11" r:id="rId10"/>
+    <sheet name="Diagnosis" sheetId="12" r:id="rId11"/>
+    <sheet name="Investigationlist" sheetId="9" r:id="rId12"/>
+    <sheet name="Allergies" sheetId="10" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="ERLinked">Investigation!$I$2:$I$3</definedName>
@@ -36,7 +37,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="202">
   <si>
     <t>PatientName</t>
   </si>
@@ -609,9 +610,6 @@
     <t>cyclenotfound</t>
   </si>
   <si>
-    <t>109</t>
-  </si>
-  <si>
     <t>Cycle Already available</t>
   </si>
   <si>
@@ -643,6 +641,18 @@
   </si>
   <si>
     <t>110</t>
+  </si>
+  <si>
+    <t>Nafisa</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>CYpFtUmzq0lITFyM0QS1gmJ7wPQZmxQCogZDfpEIbli7cnferqutf3FI9FV3MX08YQ2S71Zil5KG3a8cy9PKK1arr7zzV72dZ8JRBv32rAxC4YgjssvZrnQplz7MsMN2wC5MrSpdEZihjLoIrZWmY8Sidr999C43Hb0HxCMCQXskwiAqdZxMXTF1qpQ1xUOjWTU0pRwWu4KTnEd5xNXL0qLEHsfluMsOdaHNSamz3EnTNtjLApKgTFY5pddwNpIm</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -708,7 +718,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -734,6 +744,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,7 +1037,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -1064,41 +1078,169 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="11" max="11" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:11">
       <c r="A1" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>156</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>162</v>
+        <v>120</v>
+      </c>
+      <c r="C2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="J2" s="22">
+        <f ca="1">(TODAY() )</f>
+        <v>43262</v>
+      </c>
+      <c r="K2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="C3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3" t="s">
+        <v>190</v>
+      </c>
+      <c r="G3" t="s">
+        <v>183</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="C4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F4" t="s">
+        <v>191</v>
+      </c>
+      <c r="G4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="C5" t="s">
+        <v>171</v>
+      </c>
+      <c r="F5" t="s">
+        <v>192</v>
+      </c>
+      <c r="G5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="C6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="C7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="C8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="C9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="C10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="C11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="C12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="C13" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1108,6 +1250,51 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="38" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -1117,7 +1304,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1179,7 +1366,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:E3"/>
   <sheetViews>
@@ -1189,7 +1376,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
+    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:5">
@@ -1221,14 +1408,14 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="48.7109375" collapsed="true"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="48.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="10" customFormat="1">
@@ -1275,7 +1462,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1320,12 +1507,12 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -1380,7 +1567,7 @@
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -1398,7 +1585,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1418,7 +1605,7 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -1438,14 +1625,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="15" width="13.7109375" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" style="15" width="13.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="10.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="15" width="12.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="15" width="29.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.85546875" collapsed="true"/>
-    <col min="9" max="16384" style="15" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="13.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.85546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="15" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="14" customFormat="1">
@@ -1600,10 +1787,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="3" max="3" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
@@ -1756,6 +1943,40 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O27"/>
@@ -1766,20 +1987,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1">
@@ -2303,7 +2524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G13"/>
@@ -2314,10 +2535,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="71.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="10" customFormat="1">
@@ -2389,7 +2610,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:L8"/>
@@ -2400,11 +2621,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="4" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="38.28515625" collapsed="true"/>
+    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="38.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="10" customFormat="1">
@@ -2551,7 +2772,7 @@
         <v>124</v>
       </c>
       <c r="L6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -2579,159 +2800,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D2" t="s">
-        <v>155</v>
-      </c>
-      <c r="F2" t="s">
-        <v>190</v>
-      </c>
-      <c r="G2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="C3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D3" t="s">
-        <v>155</v>
-      </c>
-      <c r="F3" t="s">
-        <v>191</v>
-      </c>
-      <c r="G3" t="s">
-        <v>183</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="C4" t="s">
-        <v>170</v>
-      </c>
-      <c r="F4" t="s">
-        <v>192</v>
-      </c>
-      <c r="G4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="C5" t="s">
-        <v>171</v>
-      </c>
-      <c r="F5" t="s">
-        <v>193</v>
-      </c>
-      <c r="G5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="C6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="C7" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="C8" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="C9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="C10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="C11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="C12" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="C13" t="s">
-        <v>179</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
cycle listloginpagetestbase,opu cyclepage modified
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="5" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="211">
   <si>
     <t>PatientName</t>
   </si>
@@ -471,9 +471,6 @@
   </si>
   <si>
     <t xml:space="preserve">F-ICSI </t>
-  </si>
-  <si>
-    <t>8</t>
   </si>
   <si>
     <t>504 IVF SURROGACY PACKAGE</t>
@@ -607,9 +604,6 @@
     <t>sourceofsperm</t>
   </si>
   <si>
-    <t>cyclenotfound</t>
-  </si>
-  <si>
     <t>Cycle Already available</t>
   </si>
   <si>
@@ -653,6 +647,39 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>SaveMessage</t>
+  </si>
+  <si>
+    <t>Fill all mandetory fields.</t>
+  </si>
+  <si>
+    <t>Close existing cycle first.</t>
+  </si>
+  <si>
+    <t>Nilma</t>
+  </si>
+  <si>
+    <t>Record already saved.</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Cycle List</t>
+  </si>
+  <si>
+    <t>Cycle is not created or already available</t>
+  </si>
+  <si>
+    <t>Stimulation Drug</t>
+  </si>
+  <si>
+    <t>Jafari</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -1078,10 +1105,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1096,151 +1123,168 @@
     <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="16.140625" customWidth="1"/>
-    <col min="11" max="11" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="255.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>158</v>
-      </c>
       <c r="C1" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C2" t="s">
         <v>167</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="K2" t="s">
+        <v>148</v>
+      </c>
+      <c r="L2" s="22">
+        <f ca="1">(TODAY() )</f>
+        <v>43268</v>
+      </c>
+      <c r="M2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="C3" t="s">
         <v>168</v>
       </c>
-      <c r="D2" t="s">
-        <v>155</v>
-      </c>
-      <c r="F2" t="s">
-        <v>189</v>
-      </c>
-      <c r="G2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="J2" s="22">
-        <f ca="1">(TODAY() )</f>
-        <v>43262</v>
-      </c>
-      <c r="K2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="C3" t="s">
-        <v>169</v>
-      </c>
       <c r="D3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H3" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="K3" s="21" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="K3" t="s">
+        <v>201</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="C4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="K4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="C5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F5" t="s">
+        <v>190</v>
+      </c>
+      <c r="G5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="C6" t="s">
         <v>171</v>
       </c>
-      <c r="F5" t="s">
-        <v>192</v>
-      </c>
-      <c r="G5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="C6" t="s">
+    </row>
+    <row r="7" spans="1:13">
+      <c r="C7" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
-      <c r="C7" t="s">
+    <row r="8" spans="1:13">
+      <c r="C8" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
-      <c r="C8" t="s">
+    <row r="9" spans="1:13">
+      <c r="C9" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
-      <c r="C9" t="s">
+    <row r="10" spans="1:13">
+      <c r="C10" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
-      <c r="C10" t="s">
+    <row r="11" spans="1:13">
+      <c r="C11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="C11" t="s">
+    <row r="12" spans="1:13">
+      <c r="C12" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
-      <c r="C12" t="s">
+    <row r="13" spans="1:13">
+      <c r="C13" t="s">
         <v>178</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="C13" t="s">
-        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1266,26 +1310,26 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1381,7 +1425,7 @@
   <sheetData>
     <row r="1" spans="4:5">
       <c r="D1" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>66</v>
@@ -1394,7 +1438,7 @@
     </row>
     <row r="3" spans="4:5">
       <c r="E3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1406,10 +1450,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1431,7 +1475,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1462,22 +1506,28 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>198</v>
+        <v>209</v>
+      </c>
+      <c r="B7" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>182</v>
+        <v>181</v>
+      </c>
+      <c r="B8" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30">
       <c r="A9" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30">
       <c r="A10" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1502,22 +1552,22 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:1">
@@ -1552,12 +1602,12 @@
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:1">
@@ -1567,7 +1617,17 @@
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>188</v>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -1605,7 +1665,7 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -1952,7 +2012,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -2613,10 +2673,10 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2663,7 +2723,7 @@
         <v>139</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -2698,10 +2758,10 @@
         <v>123</v>
       </c>
       <c r="K2" t="s">
-        <v>142</v>
+        <v>205</v>
       </c>
       <c r="L2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -2724,7 +2784,7 @@
         <v>136</v>
       </c>
       <c r="L3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -2761,7 +2821,7 @@
         <v>130</v>
       </c>
       <c r="L5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -2772,23 +2832,34 @@
         <v>124</v>
       </c>
       <c r="L6" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="B7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C7" t="s">
         <v>125</v>
       </c>
+      <c r="L7" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="8" spans="1:12">
       <c r="B8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C8" t="s">
         <v>126</v>
+      </c>
+      <c r="L8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="L9" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
result of 26-06-2018 run
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Parag\Git\IVFmilan\src\main\java\com_Milan_TestData\"/>
     </mc:Choice>
@@ -38,7 +38,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1912" uniqueCount="1044">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1958" uniqueCount="1046">
   <si>
     <t>PatientName</t>
   </si>
@@ -3180,6 +3180,12 @@
   </si>
   <si>
     <t>OVITROP 75 IU INJ-SUN PHARMA</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
 </sst>
 </file>
@@ -3567,7 +3573,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -3616,19 +3622,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="96" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="255.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="255.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -11288,14 +11294,14 @@
   <dimension ref="A1:C116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="55.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -11930,9 +11936,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -11975,7 +11981,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -12047,7 +12053,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:5">
@@ -12085,8 +12091,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="48.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="48.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="10" customFormat="1">
@@ -12302,7 +12308,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -12342,14 +12348,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="13.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.85546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="15" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="15" width="13.7109375" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" style="15" width="13.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="10.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="15" width="12.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="15" width="29.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.8359375" collapsed="true"/>
+    <col min="9" max="16384" style="15" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="14" customFormat="1">
@@ -12504,10 +12510,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
@@ -12669,7 +12675,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -12704,20 +12710,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1">
@@ -13252,10 +13258,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="71.66796875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="10" customFormat="1">
@@ -13338,11 +13344,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="38.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="4" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="17.875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="38.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="10" customFormat="1">

</xml_diff>

<commit_message>
OPu and cyclelist pages are modified
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Parag\Git\IVFmilan\src\main\java\com_Milan_TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="1045">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1926" uniqueCount="1053">
   <si>
     <t>PatientName</t>
   </si>
@@ -3183,6 +3183,30 @@
   </si>
   <si>
     <t>Cycle Overview</t>
+  </si>
+  <si>
+    <t>Zeenath </t>
+  </si>
+  <si>
+    <t>cyclenotfound</t>
+  </si>
+  <si>
+    <t>this user has cycle saved but no package</t>
+  </si>
+  <si>
+    <t>this user has package saved but no cycle saved till 27062018</t>
+  </si>
+  <si>
+    <t>Prathyusha </t>
+  </si>
+  <si>
+    <t>New Paitent</t>
+  </si>
+  <si>
+    <t>Prathima </t>
+  </si>
+  <si>
+    <t>Add atleast 1 service.</t>
   </si>
 </sst>
 </file>
@@ -3576,12 +3600,12 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -3630,19 +3654,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="96" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="255.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.93359375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="255.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -3716,7 +3740,7 @@
       </c>
       <c r="L2" s="21">
         <f ca="1">(TODAY())</f>
-        <v>43277</v>
+        <v>43278</v>
       </c>
       <c r="M2" s="22" t="s">
         <v>925</v>
@@ -11307,10 +11331,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="55.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -11339,7 +11363,7 @@
       </c>
       <c r="D2" s="21">
         <f ca="1">(TODAY())</f>
-        <v>43277</v>
+        <v>43278</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -11964,9 +11988,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -12009,7 +12033,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -12081,7 +12105,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:5">
@@ -12111,19 +12135,20 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="48.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="48.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="54.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="10" customFormat="1">
+    <row r="1" spans="1:3" s="10" customFormat="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -12131,7 +12156,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -12139,7 +12164,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -12147,7 +12172,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -12155,25 +12180,25 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>926</v>
+        <v>1051</v>
       </c>
       <c r="B7" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>181</v>
       </c>
@@ -12181,7 +12206,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="30">
+    <row r="9" spans="1:3" ht="30">
       <c r="A9" s="1" t="s">
         <v>163</v>
       </c>
@@ -12189,7 +12214,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30">
+    <row r="10" spans="1:3" ht="30">
       <c r="A10" s="1" t="s">
         <v>164</v>
       </c>
@@ -12197,7 +12222,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -12205,7 +12230,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -12213,7 +12238,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -12221,7 +12246,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -12229,7 +12254,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>180</v>
       </c>
@@ -12237,86 +12262,116 @@
         <v>919</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
         <v>191</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
         <v>193</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>921</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>149</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>922</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="B19" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="B20" s="1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="B21" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>201</v>
       </c>
@@ -12336,7 +12391,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -12376,14 +12431,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="13.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.85546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="15" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="15" width="13.7109375" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" style="15" width="13.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="10.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="15" width="12.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="15" width="29.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.85546875" collapsed="true"/>
+    <col min="9" max="16384" style="15" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="14" customFormat="1">
@@ -12538,10 +12593,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
@@ -12703,7 +12758,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -12738,20 +12793,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1">
@@ -13286,10 +13341,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="71.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="10" customFormat="1">
@@ -13364,19 +13419,19 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="38.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="4" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="38.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="10" customFormat="1">
@@ -13448,9 +13503,6 @@
       <c r="J2" t="s">
         <v>123</v>
       </c>
-      <c r="K2" t="s">
-        <v>84</v>
-      </c>
       <c r="L2" t="s">
         <v>148</v>
       </c>
@@ -13495,7 +13547,7 @@
         <v>129</v>
       </c>
       <c r="L4" t="s">
-        <v>127</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -13534,7 +13586,7 @@
         <v>125</v>
       </c>
       <c r="L7" t="s">
-        <v>200</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -13545,12 +13597,17 @@
         <v>126</v>
       </c>
       <c r="L8" t="s">
-        <v>148</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="L9" t="s">
         <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="L10" t="s">
+        <v>1046</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes made in all pages by adding try catch block
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="5" r:id="rId1"/>
@@ -26,7 +26,8 @@
     <sheet name="Diagnosis" sheetId="12" r:id="rId12"/>
     <sheet name="InvestigationList" sheetId="9" r:id="rId13"/>
     <sheet name="Family History" sheetId="16" r:id="rId14"/>
-    <sheet name="Allergies" sheetId="10" r:id="rId15"/>
+    <sheet name="OverviewPage" sheetId="17" r:id="rId15"/>
+    <sheet name="Allergies" sheetId="10" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="ERLinked">Investigation!$I$2:$I$3</definedName>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1977" uniqueCount="1099">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1985" uniqueCount="1104">
   <si>
     <t>PatientName</t>
   </si>
@@ -3243,9 +3244,6 @@
     <t>Ritu</t>
   </si>
   <si>
-    <t>Stimulation Chart</t>
-  </si>
-  <si>
     <t>Navya </t>
   </si>
   <si>
@@ -3345,7 +3343,25 @@
     <t>Lisa</t>
   </si>
   <si>
-    <t>Akansha</t>
+    <t>Ankansha</t>
+  </si>
+  <si>
+    <t>Ishita </t>
+  </si>
+  <si>
+    <t>Cycle Overview</t>
+  </si>
+  <si>
+    <t>Noorjaha</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Nainlala </t>
+  </si>
+  <si>
+    <t>Hemlata </t>
   </si>
 </sst>
 </file>
@@ -3749,7 +3765,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3897,7 +3913,7 @@
       </c>
       <c r="L2" s="28">
         <f ca="1">(TODAY())</f>
-        <v>43288</v>
+        <v>43291</v>
       </c>
       <c r="M2" s="26"/>
       <c r="N2" s="15" t="s">
@@ -11615,7 +11631,7 @@
   <dimension ref="A1:E116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11648,18 +11664,18 @@
         <v>918</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>164</v>
       </c>
       <c r="C2" t="s">
         <v>164</v>
       </c>
       <c r="D2" s="24">
         <f ca="1">(TODAY())</f>
-        <v>43288</v>
+        <v>43291</v>
       </c>
       <c r="E2" s="25">
         <f ca="1">(TODAY())</f>
-        <v>43288</v>
+        <v>43291</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -11676,7 +11692,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>1064</v>
+        <v>1099</v>
       </c>
       <c r="B4" t="s">
         <v>921</v>
@@ -12340,10 +12356,10 @@
         <v>136</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>1090</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>1091</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -12383,7 +12399,7 @@
         <v>122</v>
       </c>
       <c r="D6" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -12391,7 +12407,7 @@
         <v>123</v>
       </c>
       <c r="D7" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -12430,16 +12446,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="7" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="D1" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="E1" t="s">
         <v>191</v>
@@ -12447,57 +12463,57 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="B2" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="C2" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="D2" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="E2" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="B3" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="C3" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="D3" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="C4" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C5" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="C6" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -12505,12 +12521,12 @@
         <v>171</v>
       </c>
       <c r="C7" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="C8" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
   </sheetData>
@@ -12521,10 +12537,39 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12542,12 +12587,12 @@
     </row>
     <row r="2" spans="4:5">
       <c r="E2" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="4:5">
       <c r="E3" s="18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -12559,7 +12604,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
@@ -12615,8 +12660,8 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>1098</v>
+      <c r="A7" s="1" t="s">
+        <v>1103</v>
       </c>
       <c r="B7" t="s">
         <v>196</v>
@@ -12624,7 +12669,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B8" t="s">
         <v>190</v>
@@ -12680,10 +12725,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>1066</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>1067</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -12840,44 +12885,70 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:3">
       <c r="B33" t="s">
         <v>1056</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:3">
       <c r="B34" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:3">
       <c r="B35" t="s">
         <v>1063</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:3">
       <c r="B36" t="s">
-        <v>1065</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="B37" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="B38" s="1" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="B39" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
         <v>1095</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="B38" s="1" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>1097</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
-        <v>1096</v>
+      <c r="C40" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="B42" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="B43" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="B44" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="B45" t="s">
+        <v>1103</v>
       </c>
     </row>
   </sheetData>
@@ -12930,7 +13001,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12994,7 +13065,7 @@
         <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>91</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="3" spans="1:8">

</xml_diff>

<commit_message>
cyclelist opu and simulationchart pages changes
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Parag\Git\IVFmilan\src\main\java\com_Milan_TestData\"/>
     </mc:Choice>
@@ -28,6 +28,7 @@
     <sheet name="Family History" sheetId="16" r:id="rId14"/>
     <sheet name="OverviewPage" sheetId="17" r:id="rId15"/>
     <sheet name="Allergies" sheetId="10" r:id="rId16"/>
+    <sheet name="ObstetricHistory" sheetId="18" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="ERLinked">Investigation!$I$2:$I$3</definedName>
@@ -40,7 +41,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1985" uniqueCount="1104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2132" uniqueCount="1113">
   <si>
     <t>PatientName</t>
   </si>
@@ -3355,13 +3356,40 @@
     <t>Noorjaha</t>
   </si>
   <si>
+    <t>Nainlala </t>
+  </si>
+  <si>
+    <t>Hemlata </t>
+  </si>
+  <si>
+    <t>Hemlata</t>
+  </si>
+  <si>
+    <t>Trusha</t>
+  </si>
+  <si>
+    <t>Trushita </t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
     <t>0</t>
   </si>
   <si>
-    <t>Nainlala </t>
-  </si>
-  <si>
-    <t>Hemlata </t>
+    <t>7</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
   </si>
 </sst>
 </file>
@@ -3770,7 +3798,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -3814,26 +3842,26 @@
   <dimension ref="A1:O1502"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="96" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="255.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.93359375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="255.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3913,7 +3941,7 @@
       </c>
       <c r="L2" s="28">
         <f ca="1">(TODAY())</f>
-        <v>43291</v>
+        <v>43293</v>
       </c>
       <c r="M2" s="26"/>
       <c r="N2" s="15" t="s">
@@ -11636,10 +11664,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="55.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="33.15234375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -11671,11 +11699,11 @@
       </c>
       <c r="D2" s="24">
         <f ca="1">(TODAY())</f>
-        <v>43291</v>
+        <v>43293</v>
       </c>
       <c r="E2" s="25">
         <f ca="1">(TODAY())</f>
-        <v>43291</v>
+        <v>43293</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -12300,9 +12328,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -12338,14 +12366,14 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1">
@@ -12439,9 +12467,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -12545,7 +12573,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -12574,7 +12602,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:5">
@@ -12593,6 +12621,30 @@
     <row r="3" spans="4:5">
       <c r="E3" s="18" t="s">
         <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="10" t="s">
+        <v>1106</v>
       </c>
     </row>
   </sheetData>
@@ -12604,17 +12656,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="48.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="48.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="54.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -12653,15 +12705,21 @@
       <c r="A5" t="s">
         <v>101</v>
       </c>
+      <c r="B5" t="s">
+        <v>1104</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>1105</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
-        <v>1103</v>
+      <c r="A7" t="s">
+        <v>1105</v>
       </c>
       <c r="B7" t="s">
         <v>196</v>
@@ -12943,12 +13001,22 @@
     </row>
     <row r="44" spans="1:3">
       <c r="B44" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="B45" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="B46" t="s">
         <v>1103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="B47" s="1" t="s">
+        <v>1104</v>
       </c>
     </row>
   </sheetData>
@@ -12966,7 +13034,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -13006,14 +13074,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="13.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.85546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="15" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="15" width="13.7109375" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" style="15" width="13.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="10.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="15" width="12.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="15" width="29.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.8359375" collapsed="true"/>
+    <col min="9" max="16384" style="15" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="14" customFormat="1">
@@ -13065,7 +13133,7 @@
         <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>1101</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -13168,10 +13236,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
@@ -13328,7 +13396,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -13363,20 +13431,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1">
@@ -13911,10 +13979,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="71.66796875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="10" customFormat="1">
@@ -13997,11 +14065,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="59.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="4" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="17.875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="59.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="10" customFormat="1">

</xml_diff>

<commit_message>
changes in addiction and homepage
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2132" uniqueCount="1113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1993" uniqueCount="1111">
   <si>
     <t>PatientName</t>
   </si>
@@ -3374,22 +3374,16 @@
     <t>count</t>
   </si>
   <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Neerali</t>
+  </si>
+  <si>
+    <t>Rashami </t>
+  </si>
+  <si>
     <t>0</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
   </si>
 </sst>
 </file>
@@ -3855,7 +3849,7 @@
     <col min="6" max="6" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="20.93359375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
     <col min="11" max="11" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
@@ -3941,7 +3935,7 @@
       </c>
       <c r="L2" s="28">
         <f ca="1">(TODAY())</f>
-        <v>43293</v>
+        <v>43296</v>
       </c>
       <c r="M2" s="26"/>
       <c r="N2" s="15" t="s">
@@ -11665,7 +11659,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="55.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="33.15234375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="33.140625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
     <col min="4" max="5" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
   </cols>
@@ -11699,11 +11693,11 @@
       </c>
       <c r="D2" s="24">
         <f ca="1">(TODAY())</f>
-        <v>43293</v>
+        <v>43296</v>
       </c>
       <c r="E2" s="25">
         <f ca="1">(TODAY())</f>
-        <v>43293</v>
+        <v>43296</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -12656,10 +12650,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12718,8 +12712,8 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>1105</v>
+      <c r="A7" s="1" t="s">
+        <v>1109</v>
       </c>
       <c r="B7" t="s">
         <v>196</v>
@@ -13017,6 +13011,16 @@
     <row r="47" spans="1:3">
       <c r="B47" s="1" t="s">
         <v>1104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="B48" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" t="s">
+        <v>1108</v>
       </c>
     </row>
   </sheetData>
@@ -13133,7 +13137,7 @@
         <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -13979,7 +13983,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="71.66796875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="71.7109375" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
@@ -14068,7 +14072,7 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
     <col min="4" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="59.5703125" collapsed="true"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
women,Obsetric and testutil classes are modified
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1993" uniqueCount="1111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2061" uniqueCount="1129">
   <si>
     <t>PatientName</t>
   </si>
@@ -3374,16 +3374,70 @@
     <t>count</t>
   </si>
   <si>
+    <t>Neerali</t>
+  </si>
+  <si>
+    <t>Rashami </t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haseena </t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
     <t>30</t>
-  </si>
-  <si>
-    <t>Neerali</t>
-  </si>
-  <si>
-    <t>Rashami </t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
 </sst>
 </file>
@@ -3841,7 +3895,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.78125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="13.85546875" collapsed="true"/>
@@ -3849,7 +3903,7 @@
     <col min="6" max="6" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.93359375" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
     <col min="11" max="11" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
@@ -3907,7 +3961,7 @@
     </row>
     <row r="2" spans="1:15" ht="30">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>202</v>
       </c>
       <c r="C2" t="s">
         <v>164</v>
@@ -3935,7 +3989,7 @@
       </c>
       <c r="L2" s="28">
         <f ca="1">(TODAY())</f>
-        <v>43296</v>
+        <v>43297</v>
       </c>
       <c r="M2" s="26"/>
       <c r="N2" s="15" t="s">
@@ -11659,7 +11713,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="55.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="33.15234375" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
     <col min="4" max="5" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
   </cols>
@@ -11686,18 +11740,18 @@
         <v>918</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>202</v>
       </c>
       <c r="C2" t="s">
         <v>164</v>
       </c>
       <c r="D2" s="24">
         <f ca="1">(TODAY())</f>
-        <v>43296</v>
+        <v>43297</v>
       </c>
       <c r="E2" s="25">
         <f ca="1">(TODAY())</f>
-        <v>43296</v>
+        <v>43297</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -12652,8 +12706,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12713,7 +12767,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="B7" t="s">
         <v>196</v>
@@ -12983,6 +13037,11 @@
         <v>1055</v>
       </c>
     </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>1108</v>
+      </c>
+    </row>
     <row r="42" spans="1:3">
       <c r="B42" t="s">
         <v>1098</v>
@@ -13020,7 +13079,7 @@
     </row>
     <row r="49" spans="2:2">
       <c r="B49" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
   </sheetData>
@@ -13137,7 +13196,7 @@
         <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>1110</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -13983,7 +14042,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="71.7109375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="71.66796875" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
@@ -14072,7 +14131,7 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
     <col min="4" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="17.875" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="59.5703125" collapsed="true"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Changes in OPU page and Obstetric history
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Parag\Git\IVFmilan\src\main\java\com_Milan_TestData\"/>
     </mc:Choice>
@@ -41,7 +41,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2061" uniqueCount="1129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1995" uniqueCount="1113">
   <si>
     <t>PatientName</t>
   </si>
@@ -3380,64 +3380,16 @@
     <t>Rashami </t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t xml:space="preserve">Haseena </t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
     <t>30</t>
+  </si>
+  <si>
+    <t>Aarasihlka </t>
+  </si>
+  <si>
+    <t>New patient</t>
   </si>
 </sst>
 </file>
@@ -3846,7 +3798,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -3895,21 +3847,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.78125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="20.93359375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="255.7109375" collapsed="true"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="96" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="255.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3989,7 +3941,7 @@
       </c>
       <c r="L2" s="28">
         <f ca="1">(TODAY())</f>
-        <v>43297</v>
+        <v>43300</v>
       </c>
       <c r="M2" s="26"/>
       <c r="N2" s="15" t="s">
@@ -11712,10 +11664,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="55.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="33.15234375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -11747,11 +11699,11 @@
       </c>
       <c r="D2" s="24">
         <f ca="1">(TODAY())</f>
-        <v>43297</v>
+        <v>43300</v>
       </c>
       <c r="E2" s="25">
         <f ca="1">(TODAY())</f>
-        <v>43297</v>
+        <v>43300</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -12376,9 +12328,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="1" max="1" width="38" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -12419,9 +12371,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1">
@@ -12515,9 +12467,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -12621,7 +12573,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -12650,7 +12602,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
+    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:5">
@@ -12687,7 +12639,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -12704,17 +12656,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="48.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="54.5703125" collapsed="true"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="48.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -12767,7 +12719,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B7" t="s">
         <v>196</v>
@@ -13077,9 +13029,17 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="49" spans="2:2">
+    <row r="49" spans="1:2">
       <c r="B49" t="s">
         <v>1107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1112</v>
       </c>
     </row>
   </sheetData>
@@ -13097,7 +13057,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -13137,14 +13097,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="15" width="13.7109375" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" style="15" width="13.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="10.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="15" width="12.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="15" width="29.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.8359375" collapsed="true"/>
-    <col min="9" max="16384" style="15" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="13.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.85546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="15" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="14" customFormat="1">
@@ -13196,7 +13156,7 @@
         <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>1128</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -13299,10 +13259,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="3" max="3" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
@@ -13459,7 +13419,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -13494,20 +13454,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1">
@@ -14042,10 +14002,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="71.66796875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="10" customFormat="1">
@@ -14128,11 +14088,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="4" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="59.5703125" collapsed="true"/>
+    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="59.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="10" customFormat="1">

</xml_diff>

<commit_message>
overview page extend report on 20072018
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Parag\Git\IVFmilan\src\main\java\com_Milan_TestData\"/>
     </mc:Choice>
@@ -41,7 +41,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1995" uniqueCount="1113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2262" uniqueCount="1130">
   <si>
     <t>PatientName</t>
   </si>
@@ -3380,16 +3380,67 @@
     <t>Rashami </t>
   </si>
   <si>
-    <t xml:space="preserve">Haseena </t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>Aarasihlka </t>
   </si>
   <si>
     <t>New patient</t>
+  </si>
+  <si>
+    <t>Haseena</t>
+  </si>
+  <si>
+    <t>84% pass percentage seen</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mrunali</t>
+  </si>
+  <si>
+    <t>79%pass for new user</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
   </si>
 </sst>
 </file>
@@ -3798,7 +3849,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -3847,21 +3898,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="96" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="255.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.93359375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="255.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3941,7 +3992,7 @@
       </c>
       <c r="L2" s="28">
         <f ca="1">(TODAY())</f>
-        <v>43300</v>
+        <v>43301</v>
       </c>
       <c r="M2" s="26"/>
       <c r="N2" s="15" t="s">
@@ -11664,10 +11715,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="55.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="33.15234375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -11692,18 +11743,18 @@
         <v>918</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>164</v>
       </c>
       <c r="C2" t="s">
         <v>164</v>
       </c>
       <c r="D2" s="24">
         <f ca="1">(TODAY())</f>
-        <v>43300</v>
+        <v>43301</v>
       </c>
       <c r="E2" s="25">
         <f ca="1">(TODAY())</f>
-        <v>43300</v>
+        <v>43301</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -12328,9 +12379,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -12371,9 +12422,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1">
@@ -12467,9 +12518,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -12573,7 +12624,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -12602,7 +12653,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:5">
@@ -12639,7 +12690,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -12656,17 +12707,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="48.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="48.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="54.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -12719,7 +12770,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>1109</v>
+        <v>1114</v>
       </c>
       <c r="B7" t="s">
         <v>196</v>
@@ -13036,10 +13087,26 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
         <v>1111</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>1112</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1115</v>
       </c>
     </row>
   </sheetData>
@@ -13057,7 +13124,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -13097,14 +13164,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="13.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.85546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="15" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="15" width="13.7109375" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" style="15" width="13.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="10.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="15" width="12.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="15" width="29.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.8359375" collapsed="true"/>
+    <col min="9" max="16384" style="15" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="14" customFormat="1">
@@ -13156,7 +13223,7 @@
         <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>1110</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -13259,10 +13326,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
@@ -13419,7 +13486,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -13454,20 +13521,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1">
@@ -14002,10 +14069,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="71.66796875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="10" customFormat="1">
@@ -14088,11 +14155,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="59.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="4" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="17.875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="59.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="10" customFormat="1">

</xml_diff>

<commit_message>
Pastmedicationhistory and sexsual history
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Parag\Git\IVFmilan\src\main\java\com_Milan_TestData\"/>
     </mc:Choice>
@@ -41,7 +41,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2262" uniqueCount="1130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2001" uniqueCount="1116">
   <si>
     <t>PatientName</t>
   </si>
@@ -3392,55 +3392,13 @@
     <t>84% pass percentage seen</t>
   </si>
   <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mrunali</t>
-  </si>
-  <si>
     <t>79%pass for new user</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>28</t>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Mrunali</t>
   </si>
 </sst>
 </file>
@@ -3849,7 +3807,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -3898,21 +3856,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="20.93359375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="255.7109375" collapsed="true"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="96" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="255.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3992,7 +3950,7 @@
       </c>
       <c r="L2" s="28">
         <f ca="1">(TODAY())</f>
-        <v>43301</v>
+        <v>43302</v>
       </c>
       <c r="M2" s="26"/>
       <c r="N2" s="15" t="s">
@@ -11715,10 +11673,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="55.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="33.15234375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -11750,11 +11708,11 @@
       </c>
       <c r="D2" s="24">
         <f ca="1">(TODAY())</f>
-        <v>43301</v>
+        <v>43302</v>
       </c>
       <c r="E2" s="25">
         <f ca="1">(TODAY())</f>
-        <v>43301</v>
+        <v>43302</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -12379,9 +12337,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="1" max="1" width="38" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -12422,9 +12380,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1">
@@ -12518,9 +12476,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -12624,7 +12582,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -12653,7 +12611,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
+    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:5">
@@ -12690,7 +12648,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -12707,17 +12665,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="48.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="54.5703125" collapsed="true"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="48.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -12770,7 +12728,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>1114</v>
+        <v>912</v>
       </c>
       <c r="B7" t="s">
         <v>196</v>
@@ -13106,7 +13064,15 @@
         <v>1109</v>
       </c>
       <c r="B52" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
         <v>1115</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1113</v>
       </c>
     </row>
   </sheetData>
@@ -13124,7 +13090,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -13164,14 +13130,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="15" width="13.7109375" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" style="15" width="13.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="10.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="15" width="12.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="15" width="29.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.8359375" collapsed="true"/>
-    <col min="9" max="16384" style="15" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="13.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.85546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="15" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="14" customFormat="1">
@@ -13223,7 +13189,7 @@
         <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -13326,10 +13292,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="3" max="3" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
@@ -13486,7 +13452,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -13521,20 +13487,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1">
@@ -14069,10 +14035,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="71.66796875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="10" customFormat="1">
@@ -14155,11 +14121,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="4" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="59.5703125" collapsed="true"/>
+    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="59.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="10" customFormat="1">

</xml_diff>

<commit_message>
changes in overview and cycle list page
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Parag\Git\IVFmilan\src\main\java\com_Milan_TestData\"/>
     </mc:Choice>
@@ -41,7 +41,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2001" uniqueCount="1116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2035" uniqueCount="1131">
   <si>
     <t>PatientName</t>
   </si>
@@ -3395,10 +3395,55 @@
     <t>79%pass for new user</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>Mrunali</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mrunali </t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
   </si>
 </sst>
 </file>
@@ -3807,7 +3852,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -3856,21 +3901,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="96" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="255.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.93359375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="255.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3922,7 +3967,7 @@
     </row>
     <row r="2" spans="1:15" ht="30">
       <c r="A2" t="s">
-        <v>202</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
         <v>164</v>
@@ -3950,7 +3995,7 @@
       </c>
       <c r="L2" s="28">
         <f ca="1">(TODAY())</f>
-        <v>43302</v>
+        <v>43303</v>
       </c>
       <c r="M2" s="26"/>
       <c r="N2" s="15" t="s">
@@ -11673,10 +11718,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="55.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -11708,11 +11753,11 @@
       </c>
       <c r="D2" s="24">
         <f ca="1">(TODAY())</f>
-        <v>43302</v>
+        <v>43303</v>
       </c>
       <c r="E2" s="25">
         <f ca="1">(TODAY())</f>
-        <v>43302</v>
+        <v>43303</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -12337,9 +12382,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -12380,9 +12425,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1">
@@ -12476,9 +12521,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -12582,7 +12627,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -12611,7 +12656,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:5">
@@ -12648,7 +12693,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -12665,17 +12710,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="48.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="48.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="54.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -12728,7 +12773,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>912</v>
+        <v>1116</v>
       </c>
       <c r="B7" t="s">
         <v>196</v>
@@ -13069,9 +13114,17 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B53" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>912</v>
+      </c>
+      <c r="B54" t="s">
         <v>1113</v>
       </c>
     </row>
@@ -13090,7 +13143,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -13130,14 +13183,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="13.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.85546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="15" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="15" width="13.7109375" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" style="15" width="13.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="10.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="15" width="12.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="15" width="29.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.8359375" collapsed="true"/>
+    <col min="9" max="16384" style="15" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="14" customFormat="1">
@@ -13189,7 +13242,7 @@
         <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -13292,10 +13345,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
@@ -13452,7 +13505,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -13487,20 +13540,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1">
@@ -14035,10 +14088,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="71.66796875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="10" customFormat="1">
@@ -14121,11 +14174,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="59.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="4" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="17.875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="59.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="10" customFormat="1">

</xml_diff>

<commit_message>
changes maded in Addictions page
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2035" uniqueCount="1131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2070" uniqueCount="1135">
   <si>
     <t>PatientName</t>
   </si>
@@ -3444,6 +3444,18 @@
   </si>
   <si>
     <t>28</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
 </sst>
 </file>
@@ -3914,7 +3926,7 @@
     <col min="11" max="11" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
     <col min="13" max="13" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.26953125" collapsed="true"/>
     <col min="15" max="15" bestFit="true" customWidth="true" width="255.7109375" collapsed="true"/>
   </cols>
   <sheetData>
@@ -13242,7 +13254,7 @@
         <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>1115</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="3" spans="1:8">

</xml_diff>

<commit_message>
util class and new run is done
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2070" uniqueCount="1135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="1138">
   <si>
     <t>PatientName</t>
   </si>
@@ -3398,54 +3398,66 @@
     <t>Mrunali</t>
   </si>
   <si>
+    <t xml:space="preserve">Mrunali </t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>90% pass percentage seen</t>
+  </si>
+  <si>
+    <t>Payal</t>
+  </si>
+  <si>
+    <t>23-Jul-2018</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
     <t>29</t>
   </si>
   <si>
-    <t xml:space="preserve">Mrunali </t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
     <t>12</t>
   </si>
   <si>
@@ -3453,9 +3465,6 @@
   </si>
   <si>
     <t>24</t>
-  </si>
-  <si>
-    <t>30</t>
   </si>
 </sst>
 </file>
@@ -4007,7 +4016,7 @@
       </c>
       <c r="L2" s="28">
         <f ca="1">(TODAY())</f>
-        <v>43303</v>
+        <v>43304</v>
       </c>
       <c r="M2" s="26"/>
       <c r="N2" s="15" t="s">
@@ -11765,11 +11774,11 @@
       </c>
       <c r="D2" s="24">
         <f ca="1">(TODAY())</f>
-        <v>43303</v>
+        <v>43304</v>
       </c>
       <c r="E2" s="25">
         <f ca="1">(TODAY())</f>
-        <v>43303</v>
+        <v>43304</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -12722,10 +12731,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12785,7 +12794,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>1116</v>
+        <v>1118</v>
       </c>
       <c r="B7" t="s">
         <v>196</v>
@@ -13138,6 +13147,14 @@
       </c>
       <c r="B54" t="s">
         <v>1113</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="1" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1117</v>
       </c>
     </row>
   </sheetData>
@@ -13254,7 +13271,7 @@
         <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>1134</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="3" spans="1:8">

</xml_diff>

<commit_message>
Made changes in pom.xml
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Parag\Git\IVFmilan\src\main\java\com_Milan_TestData\"/>
     </mc:Choice>
@@ -41,7 +41,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="1138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2006" uniqueCount="1121">
   <si>
     <t>PatientName</t>
   </si>
@@ -3407,64 +3407,13 @@
     <t>90% pass percentage seen</t>
   </si>
   <si>
+    <t>Surkha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nilma </t>
+  </si>
+  <si>
     <t>Payal</t>
-  </si>
-  <si>
-    <t>23-Jul-2018</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>24</t>
   </si>
 </sst>
 </file>
@@ -3535,7 +3484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3573,6 +3522,9 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3873,7 +3825,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -3922,21 +3874,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="20.93359375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="9.26953125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="255.7109375" collapsed="true"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="96" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="255.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -4016,7 +3968,7 @@
       </c>
       <c r="L2" s="28">
         <f ca="1">(TODAY())</f>
-        <v>43304</v>
+        <v>43306</v>
       </c>
       <c r="M2" s="26"/>
       <c r="N2" s="15" t="s">
@@ -11739,10 +11691,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="55.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="33.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -11774,11 +11726,11 @@
       </c>
       <c r="D2" s="24">
         <f ca="1">(TODAY())</f>
-        <v>43304</v>
+        <v>43306</v>
       </c>
       <c r="E2" s="25">
         <f ca="1">(TODAY())</f>
-        <v>43304</v>
+        <v>43306</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -12403,9 +12355,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="1" max="1" width="38" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -12446,9 +12398,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1">
@@ -12542,9 +12494,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -12648,7 +12600,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -12677,7 +12629,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
+    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:5">
@@ -12714,7 +12666,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -12731,17 +12683,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="48.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="54.5703125" collapsed="true"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="48.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -12797,7 +12749,7 @@
         <v>1118</v>
       </c>
       <c r="B7" t="s">
-        <v>196</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -13155,6 +13107,14 @@
       </c>
       <c r="B55" t="s">
         <v>1117</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B56" s="29">
+        <v>0.93</v>
       </c>
     </row>
   </sheetData>
@@ -13172,7 +13132,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -13212,14 +13172,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="15" width="13.7109375" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" style="15" width="13.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="10.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="15" width="12.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="15" width="29.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.8359375" collapsed="true"/>
-    <col min="9" max="16384" style="15" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="13.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.85546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="15" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="14" customFormat="1">
@@ -13374,10 +13334,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="3" max="3" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
@@ -13534,7 +13494,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -13569,20 +13529,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1">
@@ -14117,10 +14077,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="71.66796875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="10" customFormat="1">
@@ -14203,11 +14163,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="4" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="59.5703125" collapsed="true"/>
+    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="59.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="10" customFormat="1">

</xml_diff>

<commit_message>
xlsx and pom.xml is modified
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2006" uniqueCount="1121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2007" uniqueCount="1122">
   <si>
     <t>PatientName</t>
   </si>
@@ -3401,9 +3401,6 @@
     <t xml:space="preserve">Mrunali </t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>90% pass percentage seen</t>
   </si>
   <si>
@@ -3414,6 +3411,12 @@
   </si>
   <si>
     <t>Payal</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>Ishita</t>
   </si>
 </sst>
 </file>
@@ -3484,7 +3487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3525,6 +3528,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3968,7 +3972,7 @@
       </c>
       <c r="L2" s="28">
         <f ca="1">(TODAY())</f>
-        <v>43306</v>
+        <v>43307</v>
       </c>
       <c r="M2" s="26"/>
       <c r="N2" s="15" t="s">
@@ -11726,11 +11730,11 @@
       </c>
       <c r="D2" s="24">
         <f ca="1">(TODAY())</f>
-        <v>43306</v>
+        <v>43307</v>
       </c>
       <c r="E2" s="25">
         <f ca="1">(TODAY())</f>
-        <v>43306</v>
+        <v>43307</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -12683,10 +12687,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12746,10 +12750,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B7" t="s">
         <v>1118</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1119</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -13106,15 +13110,23 @@
         <v>1115</v>
       </c>
       <c r="B55" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B56" s="29">
         <v>0.93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B57" s="30">
+        <v>0.69</v>
       </c>
     </row>
   </sheetData>
@@ -13231,7 +13243,7 @@
         <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>1116</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="3" spans="1:8">

</xml_diff>

<commit_message>
allergy and complaints file updated
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2008" uniqueCount="1123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2009" uniqueCount="1124">
   <si>
     <t>PatientName</t>
   </si>
@@ -3413,13 +3413,16 @@
     <t>Payal</t>
   </si>
   <si>
-    <t>29</t>
-  </si>
-  <si>
     <t>Ishita</t>
   </si>
   <si>
     <t>Praniti</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shamita</t>
   </si>
 </sst>
 </file>
@@ -3974,7 +3977,7 @@
       </c>
       <c r="L2" s="28">
         <f ca="1">(TODAY())</f>
-        <v>43308</v>
+        <v>43309</v>
       </c>
       <c r="M2" s="26"/>
       <c r="N2" s="15" t="s">
@@ -11732,11 +11735,11 @@
       </c>
       <c r="D2" s="24">
         <f ca="1">(TODAY())</f>
-        <v>43308</v>
+        <v>43309</v>
       </c>
       <c r="E2" s="25">
         <f ca="1">(TODAY())</f>
-        <v>43308</v>
+        <v>43309</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -12689,10 +12692,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12752,7 +12755,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="B7" t="s">
         <v>1118</v>
@@ -13133,10 +13136,18 @@
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B58" s="29">
         <v>0.76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B59" s="29">
+        <v>0.84</v>
       </c>
     </row>
   </sheetData>
@@ -13253,7 +13264,7 @@
         <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>1120</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="3" spans="1:8">

</xml_diff>

<commit_message>
cycle list,overview , emr page and diagnosis page
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Parag\Git\IVFmilan\src\main\java\com_Milan_TestData\"/>
     </mc:Choice>
@@ -41,7 +41,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2009" uniqueCount="1124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2077" uniqueCount="1142">
   <si>
     <t>PatientName</t>
   </si>
@@ -3423,6 +3423,60 @@
   </si>
   <si>
     <t xml:space="preserve"> Shamita</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
 </sst>
 </file>
@@ -3834,7 +3888,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -3883,21 +3937,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="96" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="255.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.93359375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.26953125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="255.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -11700,10 +11754,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="55.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -12364,9 +12418,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -12407,9 +12461,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1">
@@ -12503,9 +12557,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -12609,7 +12663,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -12638,7 +12692,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:5">
@@ -12675,7 +12729,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -12700,9 +12754,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="48.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="48.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="54.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -13165,7 +13219,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -13205,14 +13259,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="13.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.85546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="15" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="15" width="13.7109375" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" style="15" width="13.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="10.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="15" width="12.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="15" width="29.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.8359375" collapsed="true"/>
+    <col min="9" max="16384" style="15" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="14" customFormat="1">
@@ -13264,7 +13318,7 @@
         <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>1122</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -13367,10 +13421,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
@@ -13527,7 +13581,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -13562,20 +13616,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1">
@@ -14110,10 +14164,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="71.66796875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="10" customFormat="1">
@@ -14196,11 +14250,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="59.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="4" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="17.875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="59.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="10" customFormat="1">

</xml_diff>

<commit_message>
modified testng xml and xlsx data
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2146" uniqueCount="1142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2048" uniqueCount="1139">
   <si>
     <t>PatientName</t>
   </si>
@@ -3419,40 +3419,40 @@
     <t>Praniti</t>
   </si>
   <si>
+    <t xml:space="preserve"> Shamita</t>
+  </si>
+  <si>
+    <t>Purva</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
     <t>23</t>
   </si>
   <si>
-    <t xml:space="preserve"> Shamita</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>25</t>
+    <t>24</t>
   </si>
   <si>
     <t>26</t>
@@ -3465,15 +3465,6 @@
   </si>
   <si>
     <t>29</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>24</t>
   </si>
   <si>
     <t>30</t>
@@ -3547,7 +3538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3588,6 +3579,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3945,7 +3937,7 @@
     <col min="6" max="6" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="20.93359375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
     <col min="11" max="11" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
@@ -4031,7 +4023,7 @@
       </c>
       <c r="L2" s="28">
         <f ca="1">(TODAY())</f>
-        <v>43309</v>
+        <v>43312</v>
       </c>
       <c r="M2" s="26"/>
       <c r="N2" s="15" t="s">
@@ -11789,11 +11781,11 @@
       </c>
       <c r="D2" s="24">
         <f ca="1">(TODAY())</f>
-        <v>43309</v>
+        <v>43312</v>
       </c>
       <c r="E2" s="25">
         <f ca="1">(TODAY())</f>
-        <v>43309</v>
+        <v>43312</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -12746,10 +12738,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13202,6 +13194,38 @@
       </c>
       <c r="B59" s="29">
         <v>0.84</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B60" s="29">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="1" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B61" s="29">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="1" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B62" s="30">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="1" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B63" s="29">
+        <v>0.96</v>
       </c>
     </row>
   </sheetData>
@@ -13318,7 +13342,7 @@
         <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>1141</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="3" spans="1:8">

</xml_diff>

<commit_message>
New build ran on 08082018
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Parag\Git\IVFmilan\src\main\java\com_Milan_TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2023" uniqueCount="1125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2015" uniqueCount="1127">
   <si>
     <t>PatientName</t>
   </si>
@@ -3248,9 +3248,6 @@
     <t>Navya </t>
   </si>
   <si>
-    <t>Ms.Sunanda</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Ms.Sudha </t>
   </si>
   <si>
@@ -3426,6 +3423,15 @@
   </si>
   <si>
     <t>30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abhilash </t>
+  </si>
+  <si>
+    <t>*Finalize stimulation to save OPU.</t>
+  </si>
+  <si>
+    <t>Semen Processing</t>
   </si>
 </sst>
 </file>
@@ -3838,7 +3844,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -3887,21 +3893,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="20.93359375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="255.7109375" collapsed="true"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="96" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="255.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3981,7 +3987,7 @@
       </c>
       <c r="L2" s="28">
         <f ca="1">(TODAY())</f>
-        <v>43312</v>
+        <v>43320</v>
       </c>
       <c r="M2" s="26"/>
       <c r="N2" s="15" t="s">
@@ -11699,15 +11705,15 @@
   <dimension ref="A1:E116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="55.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="33.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -11739,11 +11745,11 @@
       </c>
       <c r="D2" s="24">
         <f ca="1">(TODAY())</f>
-        <v>43312</v>
+        <v>43320</v>
       </c>
       <c r="E2" s="25">
         <f ca="1">(TODAY())</f>
-        <v>43312</v>
+        <v>43320</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -11760,7 +11766,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B4" t="s">
         <v>921</v>
@@ -11771,6 +11777,9 @@
       <c r="D4" s="21"/>
     </row>
     <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>1125</v>
+      </c>
       <c r="B5" t="s">
         <v>922</v>
       </c>
@@ -12368,9 +12377,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="1" max="1" width="38" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -12411,9 +12420,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1">
@@ -12424,10 +12433,10 @@
         <v>136</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>1088</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>1089</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>1090</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -12467,7 +12476,7 @@
         <v>122</v>
       </c>
       <c r="D6" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -12475,7 +12484,7 @@
         <v>123</v>
       </c>
       <c r="D7" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -12507,23 +12516,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="7" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="D1" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="E1" t="s">
         <v>191</v>
@@ -12531,57 +12540,57 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="B2" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="C2" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="D2" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="E2" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="B3" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="C3" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="D3" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="C4" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="C5" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C6" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -12589,12 +12598,12 @@
         <v>171</v>
       </c>
       <c r="C7" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="C8" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
   </sheetData>
@@ -12613,7 +12622,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -12642,7 +12651,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
+    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:5">
@@ -12679,12 +12688,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="10" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
   </sheetData>
@@ -12698,15 +12707,15 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="48.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="54.5703125" collapsed="true"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="48.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -12746,7 +12755,7 @@
         <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -12754,20 +12763,20 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B7" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="B8" t="s">
         <v>190</v>
@@ -12823,10 +12832,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>1065</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>1066</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -13005,25 +13014,25 @@
     </row>
     <row r="37" spans="1:3">
       <c r="B37" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="B38" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="B39" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B40" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C40" t="s">
         <v>1055</v>
@@ -13031,79 +13040,79 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="B42" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="B43" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="B44" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="B45" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="B46" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="B47" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="B48" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="B49" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B50" t="s">
         <v>1109</v>
-      </c>
-      <c r="B50" t="s">
-        <v>1110</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B51" t="s">
         <v>1111</v>
-      </c>
-      <c r="B51" t="s">
-        <v>1112</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="B52" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="B53" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -13111,20 +13120,20 @@
         <v>912</v>
       </c>
       <c r="B54" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B55" t="s">
         <v>1115</v>
-      </c>
-      <c r="B55" t="s">
-        <v>1116</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B56" s="29">
         <v>0.93</v>
@@ -13132,7 +13141,7 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="B57" s="29">
         <v>0.69</v>
@@ -13140,7 +13149,7 @@
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B58" s="29">
         <v>0.76</v>
@@ -13148,7 +13157,7 @@
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B59" s="29">
         <v>0.84</v>
@@ -13156,7 +13165,7 @@
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="B60" s="29">
         <v>0.81</v>
@@ -13164,7 +13173,7 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="B61" s="29">
         <v>0.81</v>
@@ -13172,7 +13181,7 @@
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B62" s="30">
         <v>0.81</v>
@@ -13180,7 +13189,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B63" s="29">
         <v>0.96</v>
@@ -13195,13 +13204,15 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -13222,6 +13233,11 @@
     <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>1126</v>
       </c>
     </row>
   </sheetData>
@@ -13241,14 +13257,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="15" width="13.7109375" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" style="15" width="13.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="10.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="15" width="12.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="15" width="29.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.85546875" collapsed="true"/>
-    <col min="9" max="16384" style="15" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="13.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.85546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="15" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="14" customFormat="1">
@@ -13300,7 +13316,7 @@
         <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -13403,10 +13419,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="3" max="3" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
@@ -13563,7 +13579,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -13598,20 +13614,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1">
@@ -14146,10 +14162,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="71.66796875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="10" customFormat="1">
@@ -14232,11 +14248,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="4" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="59.5703125" collapsed="true"/>
+    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="59.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="10" customFormat="1">

</xml_diff>

<commit_message>
Testbase class is modified after buildfailure
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Parag\Git\IVFmilan\src\main\java\com_Milan_TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="11" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="5" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="OverviewPage" sheetId="17" r:id="rId15"/>
     <sheet name="Allergies" sheetId="10" r:id="rId16"/>
     <sheet name="ObstetricHistory" sheetId="18" r:id="rId17"/>
+    <sheet name="SiemenProcessing" sheetId="19" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="ERLinked">Investigation!$I$2:$I$3</definedName>
@@ -41,7 +42,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2015" uniqueCount="1127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="1129">
   <si>
     <t>PatientName</t>
   </si>
@@ -3432,6 +3433,12 @@
   </si>
   <si>
     <t>Semen Processing</t>
+  </si>
+  <si>
+    <t>Progressive</t>
+  </si>
+  <si>
+    <t>NonProgressive</t>
   </si>
 </sst>
 </file>
@@ -3844,7 +3851,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="40.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -3893,21 +3900,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="96" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="255.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.26953125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="255.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -3987,7 +3994,7 @@
       </c>
       <c r="L2" s="28">
         <f ca="1">(TODAY())</f>
-        <v>43320</v>
+        <v>43321</v>
       </c>
       <c r="M2" s="26"/>
       <c r="N2" s="15" t="s">
@@ -11710,10 +11717,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="55.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -11745,11 +11752,11 @@
       </c>
       <c r="D2" s="24">
         <f ca="1">(TODAY())</f>
-        <v>43320</v>
+        <v>43321</v>
       </c>
       <c r="E2" s="25">
         <f ca="1">(TODAY())</f>
-        <v>43320</v>
+        <v>43321</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -12377,9 +12384,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -12420,9 +12427,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1">
@@ -12516,9 +12523,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -12622,7 +12629,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -12651,7 +12658,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="53.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:5">
@@ -12688,7 +12695,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -12699,6 +12706,81 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="17" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>60</v>
+      </c>
+      <c r="B4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>60</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>55</v>
+      </c>
+      <c r="B6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>80</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -12713,9 +12795,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="48.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="48.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="54.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1">
@@ -13206,13 +13288,13 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -13257,14 +13339,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.7109375" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="13.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.85546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.85546875" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="15" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="15" width="13.7109375" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" style="15" width="13.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="10.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="15" width="12.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="15" width="29.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.85546875" collapsed="true"/>
+    <col min="9" max="16384" style="15" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="14" customFormat="1">
@@ -13419,10 +13501,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1">
@@ -13579,7 +13661,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -13614,20 +13696,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1">
@@ -14162,10 +14244,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="71.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="71.66796875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="10" customFormat="1">
@@ -14248,11 +14330,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="59.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="4" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="59.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="10" customFormat="1">

</xml_diff>

<commit_message>
SiemensProcessing , Siemensdetails and Menstrualhistory page is modified
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="1129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2088" uniqueCount="1145">
   <si>
     <t>PatientName</t>
   </si>
@@ -3439,6 +3439,54 @@
   </si>
   <si>
     <t>NonProgressive</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
   </si>
 </sst>
 </file>
@@ -13345,7 +13393,7 @@
     <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="10.28515625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="15" width="12.0" collapsed="true"/>
     <col min="7" max="7" customWidth="true" style="15" width="29.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.8359375" collapsed="true"/>
     <col min="9" max="16384" style="15" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Modified testbase class by adding 64 version chrome diver exe
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2035" uniqueCount="1131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2052" uniqueCount="1131">
   <si>
     <t>PatientName</t>
   </si>
@@ -3919,7 +3919,7 @@
     <col min="11" max="11" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
     <col min="13" max="13" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.26953125" collapsed="true"/>
     <col min="15" max="15" bestFit="true" customWidth="true" width="255.7109375" collapsed="true"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Ivf latest run result-97%
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2085" uniqueCount="1131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2116" uniqueCount="1150">
   <si>
     <t>PatientName</t>
   </si>
@@ -3417,34 +3417,91 @@
     <t>Purva</t>
   </si>
   <si>
+    <t xml:space="preserve">Abhilash </t>
+  </si>
+  <si>
+    <t>*Finalize stimulation to save OPU.</t>
+  </si>
+  <si>
+    <t>Semen Processing</t>
+  </si>
+  <si>
+    <t>Progressive</t>
+  </si>
+  <si>
+    <t>NonProgressive</t>
+  </si>
+  <si>
+    <t>Ms.Nandini </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nandini </t>
+  </si>
+  <si>
+    <t>Ms.Nandini</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>Asmita</t>
+  </si>
+  <si>
+    <t>gAYATRI</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
     <t>30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abhilash </t>
-  </si>
-  <si>
-    <t>*Finalize stimulation to save OPU.</t>
-  </si>
-  <si>
-    <t>Semen Processing</t>
-  </si>
-  <si>
-    <t>Progressive</t>
-  </si>
-  <si>
-    <t>NonProgressive</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gayatri</t>
-  </si>
-  <si>
-    <t>Ms.Nandini </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nandini </t>
-  </si>
-  <si>
-    <t>Ms.Nandini</t>
   </si>
 </sst>
 </file>
@@ -4000,7 +4057,7 @@
       </c>
       <c r="L2" s="28">
         <f ca="1">(TODAY())</f>
-        <v>43327</v>
+        <v>43335</v>
       </c>
       <c r="M2" s="26"/>
       <c r="N2" s="15" t="s">
@@ -11758,11 +11815,11 @@
       </c>
       <c r="D2" s="24">
         <f ca="1">(TODAY())</f>
-        <v>43327</v>
+        <v>43335</v>
       </c>
       <c r="E2" s="25">
         <f ca="1">(TODAY())</f>
-        <v>43327</v>
+        <v>43335</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -11791,7 +11848,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B5" t="s">
         <v>921</v>
@@ -12731,10 +12788,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="17" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>1125</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>1126</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -12793,10 +12850,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12856,7 +12913,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>1127</v>
+        <v>1130</v>
       </c>
       <c r="B7" t="s">
         <v>1115</v>
@@ -12864,7 +12921,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="B8" t="s">
         <v>189</v>
@@ -12920,7 +12977,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1064</v>
@@ -12928,7 +12985,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>911</v>
@@ -13291,9 +13348,17 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>1128</v>
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="1" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B66" s="30">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
@@ -13338,7 +13403,7 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
   </sheetData>
@@ -13364,7 +13429,7 @@
     <col min="5" max="5" bestFit="true" customWidth="true" style="15" width="10.28515625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="15" width="12.0" collapsed="true"/>
     <col min="7" max="7" customWidth="true" style="15" width="29.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="15" width="8.8359375" collapsed="true"/>
     <col min="9" max="16384" style="15" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
@@ -13417,7 +13482,7 @@
         <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>1121</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="3" spans="1:8">

</xml_diff>

<commit_message>
Female report page is modified
</commit_message>
<xml_diff>
--- a/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
+++ b/IVFmilan/src/main/java/com_Milan_TestData/Milandata.xlsx
@@ -9,27 +9,28 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="4590" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="5" r:id="rId1"/>
     <sheet name="HomePage" sheetId="1" r:id="rId2"/>
-    <sheet name="EMRPage" sheetId="7" r:id="rId3"/>
-    <sheet name="Addictions" sheetId="6" r:id="rId4"/>
-    <sheet name="Vitals" sheetId="2" r:id="rId5"/>
-    <sheet name="Complaints" sheetId="13" r:id="rId6"/>
-    <sheet name="SexualHistory" sheetId="3" r:id="rId7"/>
-    <sheet name="pastMedicationHistory" sheetId="4" r:id="rId8"/>
-    <sheet name="Investigation" sheetId="8" r:id="rId9"/>
-    <sheet name="CycleList" sheetId="11" r:id="rId10"/>
-    <sheet name="Stimulationchart" sheetId="14" r:id="rId11"/>
-    <sheet name="Diagnosis" sheetId="12" r:id="rId12"/>
-    <sheet name="InvestigationList" sheetId="9" r:id="rId13"/>
-    <sheet name="Family History" sheetId="16" r:id="rId14"/>
-    <sheet name="OverviewPage" sheetId="17" r:id="rId15"/>
-    <sheet name="Allergies" sheetId="10" r:id="rId16"/>
-    <sheet name="ObstetricHistory" sheetId="18" r:id="rId17"/>
-    <sheet name="SiemenProcessing" sheetId="19" r:id="rId18"/>
+    <sheet name="FemaleReportUpload" sheetId="21" r:id="rId3"/>
+    <sheet name="EMRPage" sheetId="7" r:id="rId4"/>
+    <sheet name="Addictions" sheetId="6" r:id="rId5"/>
+    <sheet name="Vitals" sheetId="2" r:id="rId6"/>
+    <sheet name="Complaints" sheetId="13" r:id="rId7"/>
+    <sheet name="SexualHistory" sheetId="3" r:id="rId8"/>
+    <sheet name="pastMedicationHistory" sheetId="4" r:id="rId9"/>
+    <sheet name="Investigation" sheetId="8" r:id="rId10"/>
+    <sheet name="CycleList" sheetId="11" r:id="rId11"/>
+    <sheet name="Stimulationchart" sheetId="14" r:id="rId12"/>
+    <sheet name="Diagnosis" sheetId="12" r:id="rId13"/>
+    <sheet name="InvestigationList" sheetId="9" r:id="rId14"/>
+    <sheet name="Family History" sheetId="16" r:id="rId15"/>
+    <sheet name="OverviewPage" sheetId="17" r:id="rId16"/>
+    <sheet name="Allergies" sheetId="10" r:id="rId17"/>
+    <sheet name="ObstetricHistory" sheetId="18" r:id="rId18"/>
+    <sheet name="SiemenProcessing" sheetId="19" r:id="rId19"/>
   </sheets>
   <definedNames>
     <definedName name="ERLinked">Investigation!$I$2:$I$3</definedName>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="1137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2038" uniqueCount="1148">
   <si>
     <t>PatientName</t>
   </si>
@@ -3463,6 +3464,39 @@
   </si>
   <si>
     <t>Nilima</t>
+  </si>
+  <si>
+    <t>Laboratory</t>
+  </si>
+  <si>
+    <t>Radiology</t>
+  </si>
+  <si>
+    <t>Procedure</t>
+  </si>
+  <si>
+    <t>Pre Anesthesia</t>
+  </si>
+  <si>
+    <t>Report Category</t>
+  </si>
+  <si>
+    <t>Lab</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>Proce</t>
+  </si>
+  <si>
+    <t>PreAnesthesia</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>ReportName</t>
   </si>
 </sst>
 </file>
@@ -3924,6 +3958,219 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet8"/>
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="59.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="10" customFormat="1">
+      <c r="A1" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" t="s">
+        <v>118</v>
+      </c>
+      <c r="J2" t="s">
+        <v>119</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="L2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="B3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I3" t="s">
+        <v>132</v>
+      </c>
+      <c r="L3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="B4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H4" t="s">
+        <v>125</v>
+      </c>
+      <c r="L4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="B5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" t="s">
+        <v>136</v>
+      </c>
+      <c r="H5" t="s">
+        <v>126</v>
+      </c>
+      <c r="L5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="L6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="B7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" t="s">
+        <v>121</v>
+      </c>
+      <c r="L7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="B8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" t="s">
+        <v>122</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="L9" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="L10" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="L11" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+      <formula1>"package+$A$10"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1502"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
@@ -3945,7 +4192,7 @@
     <col min="11" max="11" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="255.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -4026,7 +4273,7 @@
       </c>
       <c r="L2" s="28">
         <f ca="1">(TODAY())</f>
-        <v>43350</v>
+        <v>43355</v>
       </c>
       <c r="M2" s="26"/>
       <c r="N2" s="15" t="s">
@@ -11739,7 +11986,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E116"/>
   <sheetViews>
@@ -11784,11 +12031,11 @@
       </c>
       <c r="D2" s="24">
         <f ca="1">(TODAY())</f>
-        <v>43350</v>
+        <v>43355</v>
       </c>
       <c r="E2" s="25">
         <f ca="1">(TODAY())</f>
-        <v>43350</v>
+        <v>43355</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -12412,7 +12659,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -12455,7 +12702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -12551,7 +12798,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -12657,7 +12904,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -12686,7 +12933,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:E3"/>
   <sheetViews>
@@ -12723,7 +12970,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -12747,7 +12994,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -12827,8 +13074,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13355,11 +13602,79 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="9" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13398,7 +13713,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:H6"/>
@@ -13560,7 +13875,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G6"/>
@@ -13721,7 +14036,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -13755,7 +14070,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O27"/>
@@ -14303,7 +14618,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G13"/>
@@ -14387,217 +14702,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:L11"/>
-  <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="10" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="59.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" s="10" customFormat="1">
-      <c r="A1" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H2" t="s">
-        <v>131</v>
-      </c>
-      <c r="I2" t="s">
-        <v>118</v>
-      </c>
-      <c r="J2" t="s">
-        <v>119</v>
-      </c>
-      <c r="K2" t="s">
-        <v>1039</v>
-      </c>
-      <c r="L2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="B3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E3" t="s">
-        <v>128</v>
-      </c>
-      <c r="H3" t="s">
-        <v>124</v>
-      </c>
-      <c r="I3" t="s">
-        <v>132</v>
-      </c>
-      <c r="L3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="B4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" t="s">
-        <v>129</v>
-      </c>
-      <c r="H4" t="s">
-        <v>125</v>
-      </c>
-      <c r="L4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="B5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D5" t="s">
-        <v>136</v>
-      </c>
-      <c r="H5" t="s">
-        <v>126</v>
-      </c>
-      <c r="L5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="B6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L6" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="B7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C7" t="s">
-        <v>121</v>
-      </c>
-      <c r="L7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="B8" t="s">
-        <v>141</v>
-      </c>
-      <c r="C8" t="s">
-        <v>122</v>
-      </c>
-      <c r="L8" t="s">
-        <v>1038</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="L9" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="L10" t="s">
-        <v>1032</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="L11" t="s">
-        <v>1044</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
-      <formula1>"package+$A$10"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>